<commit_message>
16° Commit : Aggiornamento delle patch e dei trattamenti di core ( Elem di X3  & trattamenti)
</commit_message>
<xml_diff>
--- a/table/tableList_protocolCore.xlsx
+++ b/table/tableList_protocolCore.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcorbara\Documents\ArgoX3_API_Mobile_CORE\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A0D2C4-BC40-4AA8-8140-E3246FDA6832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6D5AE0-B12E-474D-8238-E7B060432349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nuove tabelle" sheetId="1" r:id="rId1"/>
@@ -389,7 +389,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,12 +399,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -725,23 +719,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1024,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1210,7 +1195,7 @@
       <c r="J8" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="51"/>
+      <c r="K8" s="54"/>
     </row>
     <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H9" s="34" t="s">
@@ -1222,7 +1207,7 @@
       <c r="J9" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="51"/>
+      <c r="K9" s="54"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1234,8 +1219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C6CAB61-4E19-4D48-B29B-AF9E6005A9F4}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2038,35 +2023,35 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="41"/>
-      <c r="B27" s="57" t="s">
+      <c r="B27" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="54" t="s">
+      <c r="C27" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" s="54">
+      <c r="D27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="4">
         <v>50</v>
       </c>
-      <c r="F27" s="56" t="s">
-        <v>95</v>
-      </c>
-      <c r="G27" s="53">
+      <c r="F27" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="G27" s="6">
         <v>1</v>
       </c>
-      <c r="H27" s="53" t="s">
+      <c r="H27" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="I27" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="J27" s="54"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="54"/>
-      <c r="M27" s="54"/>
-      <c r="N27" s="55"/>
+      <c r="I27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="52"/>
     </row>
     <row r="28" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="34"/>
@@ -2186,7 +2171,7 @@
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="51" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="38" t="s">

</xml_diff>